<commit_message>
notebooks ratiometric y notebooks entropía
</commit_message>
<xml_diff>
--- a/Promedios réplicas todo/valores de alfa y rho todo.xlsx
+++ b/Promedios réplicas todo/valores de alfa y rho todo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8640" windowHeight="4200" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8640" windowHeight="4200" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="J23101 RFP Y pLux76 RFP" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="87">
   <si>
     <t xml:space="preserve">control gluc </t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>promedio</t>
+  </si>
+  <si>
+    <t>rho RFP 2</t>
+  </si>
+  <si>
+    <t>rho YFP 2</t>
   </si>
 </sst>
 </file>
@@ -831,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M29"/>
+  <dimension ref="A2:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26:K26"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1604,9 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1607,24 +1615,232 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="K28" s="3"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2">
+        <v>-0.45840925999999999</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.12875244999999999</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.17326108000000001</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.24748328999999999</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.1514789</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.23671253</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.13153129999999999</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.17592653</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.6394976</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0.28558742999999998</v>
+      </c>
       <c r="L29" s="3"/>
       <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>-0.73338448000000001</v>
+      </c>
+      <c r="C30">
+        <v>0.1061735</v>
+      </c>
+      <c r="D30">
+        <v>0.21143096</v>
+      </c>
+      <c r="E30">
+        <v>0.27713815000000003</v>
+      </c>
+      <c r="F30">
+        <v>0.17476248</v>
+      </c>
+      <c r="G30">
+        <v>0.23950163999999999</v>
+      </c>
+      <c r="H30">
+        <v>0.13268374999999999</v>
+      </c>
+      <c r="I30">
+        <v>0.18960144000000001</v>
+      </c>
+      <c r="J30">
+        <v>0.58975504999999995</v>
+      </c>
+      <c r="K30">
+        <v>0.32414767999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31">
+        <v>-0.25898706999999999</v>
+      </c>
+      <c r="C31">
+        <v>-0.22929289999999999</v>
+      </c>
+      <c r="D31">
+        <v>0.22826046999999999</v>
+      </c>
+      <c r="E31">
+        <v>0.26625854999999998</v>
+      </c>
+      <c r="F31">
+        <v>0.18139717</v>
+      </c>
+      <c r="G31">
+        <v>0.17168997999999999</v>
+      </c>
+      <c r="H31">
+        <v>0.14135955</v>
+      </c>
+      <c r="I31">
+        <v>0.12765048000000001</v>
+      </c>
+      <c r="J31">
+        <v>0.53444758999999997</v>
+      </c>
+      <c r="K31">
+        <v>0.15417249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>-2.18145678</v>
+      </c>
+      <c r="C34">
+        <v>7.7668426000000004</v>
+      </c>
+      <c r="D34">
+        <v>5.7716365700000001</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4.0406768700000004</v>
+      </c>
+      <c r="F34">
+        <v>6.6015796</v>
+      </c>
+      <c r="G34">
+        <v>4.2245333599999997</v>
+      </c>
+      <c r="H34">
+        <v>7.6027528599999998</v>
+      </c>
+      <c r="I34">
+        <v>5.6841910100000002</v>
+      </c>
+      <c r="J34">
+        <v>1.56372752</v>
+      </c>
+      <c r="K34">
+        <v>3.5015546799999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>-1.3635412600000001</v>
+      </c>
+      <c r="C35">
+        <v>9.4185464799999998</v>
+      </c>
+      <c r="D35">
+        <v>4.7296762399999999</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3.6083087699999998</v>
+      </c>
+      <c r="F35">
+        <v>5.7220519799999998</v>
+      </c>
+      <c r="G35">
+        <v>4.17533669</v>
+      </c>
+      <c r="H35">
+        <v>7.5367182100000001</v>
+      </c>
+      <c r="I35">
+        <v>5.2742214499999998</v>
+      </c>
+      <c r="J35">
+        <v>1.69561922</v>
+      </c>
+      <c r="K35">
+        <v>3.0850135700000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <v>-3.8611966099999999</v>
+      </c>
+      <c r="C36">
+        <v>-4.3612339799999997</v>
+      </c>
+      <c r="D36">
+        <v>4.3809600299999998</v>
+      </c>
+      <c r="E36" s="1">
+        <v>3.7557478899999999</v>
+      </c>
+      <c r="F36">
+        <v>5.51276528</v>
+      </c>
+      <c r="G36">
+        <v>5.8244516700000002</v>
+      </c>
+      <c r="H36">
+        <v>7.0741593099999998</v>
+      </c>
+      <c r="I36">
+        <v>7.83389164</v>
+      </c>
+      <c r="J36">
+        <v>1.87109087</v>
+      </c>
+      <c r="K36">
+        <v>6.4862415499999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E37" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3069,10 +3285,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M29"/>
+  <dimension ref="A2:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26:K26"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3827,31 +4043,263 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="3"/>
+      <c r="A29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2">
+        <v>-0.28272129000000001</v>
+      </c>
+      <c r="C29" s="2">
+        <v>-0.16508431000000001</v>
+      </c>
+      <c r="D29">
+        <v>7.3186840000000003E-2</v>
+      </c>
+      <c r="E29">
+        <v>8.5866919999999999E-2</v>
+      </c>
+      <c r="F29">
+        <v>0.6970944</v>
+      </c>
+      <c r="G29">
+        <v>0.86300484</v>
+      </c>
+      <c r="H29">
+        <v>0.34496135999999999</v>
+      </c>
+      <c r="I29">
+        <v>9.829214E-2</v>
+      </c>
+      <c r="J29">
+        <v>0.33955464000000002</v>
+      </c>
+      <c r="K29">
+        <v>9.6687869999999995E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>-0.26702429</v>
+      </c>
+      <c r="C30">
+        <v>-0.25354545000000001</v>
+      </c>
+      <c r="D30">
+        <v>7.9411659999999995E-2</v>
+      </c>
+      <c r="E30">
+        <v>8.7319220000000003E-2</v>
+      </c>
+      <c r="F30">
+        <v>0.71329138000000003</v>
+      </c>
+      <c r="G30">
+        <v>0.91412391000000004</v>
+      </c>
+      <c r="H30">
+        <v>0.35405135999999998</v>
+      </c>
+      <c r="I30">
+        <v>0.10155146</v>
+      </c>
+      <c r="J30">
+        <v>0.36209795</v>
+      </c>
+      <c r="K30">
+        <v>0.11815607</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31">
+        <v>-0.65779032999999998</v>
+      </c>
+      <c r="C31">
+        <v>-0.14382376999999999</v>
+      </c>
+      <c r="D31">
+        <v>2.8076940000000002E-2</v>
+      </c>
+      <c r="E31">
+        <v>9.3459429999999996E-2</v>
+      </c>
+      <c r="F31">
+        <v>0.62393960999999998</v>
+      </c>
+      <c r="G31">
+        <v>1.0799983500000001</v>
+      </c>
+      <c r="H31">
+        <v>0.27715916000000002</v>
+      </c>
+      <c r="I31">
+        <v>0.12306048999999999</v>
+      </c>
+      <c r="J31">
+        <v>0.24235841</v>
+      </c>
+      <c r="K31">
+        <v>0.12074482</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>-3.5370523899999999</v>
+      </c>
+      <c r="C34">
+        <v>-6.0575107499999996</v>
+      </c>
+      <c r="D34">
+        <v>13.66365854</v>
+      </c>
+      <c r="E34" s="1">
+        <v>11.645927929999999</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1.4345259400000001</v>
+      </c>
+      <c r="G34">
+        <v>1.1587420500000001</v>
+      </c>
+      <c r="H34">
+        <v>2.8988753699999998</v>
+      </c>
+      <c r="I34">
+        <v>10.173753870000001</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2.9450341299999998</v>
+      </c>
+      <c r="K34">
+        <v>10.34255851</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>-3.74497766</v>
+      </c>
+      <c r="C35">
+        <v>-3.9440660699999999</v>
+      </c>
+      <c r="D35">
+        <v>12.59260944</v>
+      </c>
+      <c r="E35" s="1">
+        <v>11.452231749999999</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1.4019516000000001</v>
+      </c>
+      <c r="G35">
+        <v>1.0939436</v>
+      </c>
+      <c r="H35">
+        <v>2.8244489800000001</v>
+      </c>
+      <c r="I35">
+        <v>9.8472244199999999</v>
+      </c>
+      <c r="J35">
+        <v>2.7616836500000002</v>
+      </c>
+      <c r="K35">
+        <v>8.4633821200000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <v>-1.5202412700000001</v>
+      </c>
+      <c r="C36">
+        <v>-6.9529536600000004</v>
+      </c>
+      <c r="D36">
+        <v>35.616423230000002</v>
+      </c>
+      <c r="E36" s="1">
+        <v>10.69983032</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1.6027192100000001</v>
+      </c>
+      <c r="G36">
+        <v>0.92592733999999999</v>
+      </c>
+      <c r="H36">
+        <v>3.60803517</v>
+      </c>
+      <c r="I36">
+        <v>8.1260847300000005</v>
+      </c>
+      <c r="J36">
+        <v>4.1261204500000002</v>
+      </c>
+      <c r="K36">
+        <v>8.2819286900000009</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3863,8 +4311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4649,7 +5097,9 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -4658,141 +5108,239 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="K28" s="3"/>
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2">
+        <v>-0.64102201000000003</v>
+      </c>
+      <c r="C29" s="2">
+        <v>-0.19468515</v>
+      </c>
+      <c r="D29" s="2">
+        <v>8.0067840000000001E-2</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.11217303000000001</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.31064089</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.43334470000000003</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.49865092</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.16355228999999999</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.70209942999999997</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1.1356954100000001</v>
+      </c>
+      <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>-0.50129360000000001</v>
+      </c>
+      <c r="C30">
+        <v>-0.13231994999999999</v>
+      </c>
+      <c r="D30">
+        <v>7.1474410000000002E-2</v>
+      </c>
+      <c r="E30">
+        <v>0.12526092</v>
+      </c>
+      <c r="F30">
+        <v>0.27719839000000002</v>
+      </c>
+      <c r="G30">
+        <v>0.45166687</v>
+      </c>
+      <c r="H30">
+        <v>0.44841577999999999</v>
+      </c>
+      <c r="I30">
+        <v>0.17582840999999999</v>
+      </c>
+      <c r="J30">
+        <v>0.68419322000000005</v>
+      </c>
+      <c r="K30">
+        <v>1.2543506</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31">
+        <v>-0.54957515999999995</v>
+      </c>
+      <c r="C31">
+        <v>-0.15864017999999999</v>
+      </c>
+      <c r="D31">
+        <v>7.6055200000000003E-2</v>
+      </c>
+      <c r="E31">
+        <v>0.11580097</v>
+      </c>
+      <c r="F31">
+        <v>0.28099521999999999</v>
+      </c>
+      <c r="G31">
+        <v>0.47386507999999999</v>
+      </c>
+      <c r="H31">
+        <v>0.39802486999999998</v>
+      </c>
+      <c r="I31">
+        <v>0.18133394999999999</v>
+      </c>
+      <c r="J31">
+        <v>0.66422685999999997</v>
+      </c>
+      <c r="K31">
+        <v>1.1399930599999999</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>-1.56000885</v>
+      </c>
+      <c r="C34">
+        <v>-5.1364986200000002</v>
+      </c>
+      <c r="D34">
+        <v>12.48940867</v>
+      </c>
+      <c r="E34" s="1">
+        <v>8.9147989899999995</v>
+      </c>
+      <c r="F34">
+        <v>3.21915124</v>
+      </c>
+      <c r="G34">
+        <v>2.30763176</v>
+      </c>
+      <c r="H34">
+        <v>2.0054109200000001</v>
+      </c>
+      <c r="I34">
+        <v>6.1142524700000003</v>
+      </c>
+      <c r="J34" s="1">
+        <v>1.42429969</v>
+      </c>
+      <c r="K34">
+        <v>0.88051778000000003</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>-1.9948389399999999</v>
+      </c>
+      <c r="C35">
+        <v>-7.5574395599999997</v>
+      </c>
+      <c r="D35">
+        <v>13.9910216</v>
+      </c>
+      <c r="E35" s="1">
+        <v>7.9833358099999998</v>
+      </c>
+      <c r="F35">
+        <v>3.6075245300000001</v>
+      </c>
+      <c r="G35">
+        <v>2.21402112</v>
+      </c>
+      <c r="H35">
+        <v>2.2300731499999999</v>
+      </c>
+      <c r="I35">
+        <v>5.6873629799999996</v>
+      </c>
+      <c r="J35">
+        <v>1.4615754299999999</v>
+      </c>
+      <c r="K35">
+        <v>0.79722528000000004</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <v>-1.81958734</v>
+      </c>
+      <c r="C36">
+        <v>-6.3035732900000001</v>
+      </c>
+      <c r="D36">
+        <v>13.1483457</v>
+      </c>
+      <c r="E36" s="1">
+        <v>8.6355064099999996</v>
+      </c>
+      <c r="F36">
+        <v>3.5587793699999999</v>
+      </c>
+      <c r="G36">
+        <v>2.11030534</v>
+      </c>
+      <c r="H36">
+        <v>2.5124058100000002</v>
+      </c>
+      <c r="I36">
+        <v>5.5146872599999996</v>
+      </c>
+      <c r="J36">
+        <v>1.50550973</v>
+      </c>
+      <c r="K36">
+        <v>0.87719831999999998</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
+      <c r="E37" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="E38" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -4806,7 +5354,6 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -4820,7 +5367,9 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="E40" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -4834,7 +5383,9 @@
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="E41" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -4848,7 +5399,6 @@
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -4862,7 +5412,9 @@
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="E43" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -5419,6 +5971,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5426,8 +5979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M154"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6168,7 +6721,9 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -6180,49 +6735,114 @@
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2">
+        <v>-0.24467341000000001</v>
+      </c>
+      <c r="C29" s="2">
+        <v>-0.22982280999999999</v>
+      </c>
+      <c r="D29" s="2">
+        <v>5.9861030000000003E-2</v>
+      </c>
+      <c r="E29" s="2">
+        <v>9.6440540000000005E-2</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.19041101999999999</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.28478576999999999</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.23684231</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.16077370999999999</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.55008584999999999</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0.84450459</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>-0.43088309000000002</v>
+      </c>
+      <c r="C30">
+        <v>-0.14245415</v>
+      </c>
+      <c r="D30" s="2">
+        <v>6.2855300000000003E-2</v>
+      </c>
+      <c r="E30" s="2">
+        <v>8.5873690000000003E-2</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.21413315999999999</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.28786676</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.28871047999999999</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0.21478195999999999</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0.65099149000000001</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.95314144999999995</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31">
+        <v>-0.36049350000000002</v>
+      </c>
+      <c r="C31">
+        <v>-6.759424E-2</v>
+      </c>
+      <c r="D31" s="2">
+        <v>5.7619869999999997E-2</v>
+      </c>
+      <c r="E31" s="2">
+        <v>8.7736969999999997E-2</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.19893058999999999</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.28450721000000001</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.26911051000000002</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0.11140904</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0.60146082999999995</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0.94719140999999996</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -6232,10 +6852,12 @@
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -6245,48 +6867,111 @@
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>-4.0870807500000002</v>
+      </c>
+      <c r="C34">
+        <v>-4.3511782200000004</v>
+      </c>
+      <c r="D34" s="1">
+        <v>16.705359040000001</v>
+      </c>
+      <c r="E34" s="1">
+        <v>10.369082840000001</v>
+      </c>
+      <c r="F34" s="2">
+        <v>5.2517967900000002</v>
+      </c>
+      <c r="G34" s="2">
+        <v>3.5114114000000001</v>
+      </c>
+      <c r="H34" s="2">
+        <v>4.2222186300000004</v>
+      </c>
+      <c r="I34" s="2">
+        <v>6.2199223999999997</v>
+      </c>
+      <c r="J34" s="1">
+        <v>1.8178980600000001</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1.18412619</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>-2.3208151300000002</v>
+      </c>
+      <c r="C35">
+        <v>-7.01980249</v>
+      </c>
+      <c r="D35" s="1">
+        <v>15.909556970000001</v>
+      </c>
+      <c r="E35" s="2">
+        <v>11.64501074</v>
+      </c>
+      <c r="F35" s="2">
+        <v>4.6699913899999999</v>
+      </c>
+      <c r="G35" s="2">
+        <v>3.47382934</v>
+      </c>
+      <c r="H35" s="2">
+        <v>3.4636775399999999</v>
+      </c>
+      <c r="I35" s="2">
+        <v>4.6558844099999996</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1.5361183899999999</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1.0491622199999999</v>
+      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <v>-2.7739751500000001</v>
+      </c>
+      <c r="C36">
+        <v>-14.794159430000001</v>
+      </c>
+      <c r="D36" s="1">
+        <v>17.3551252</v>
+      </c>
+      <c r="E36" s="2">
+        <v>11.397703529999999</v>
+      </c>
+      <c r="F36" s="2">
+        <v>5.0268790799999996</v>
+      </c>
+      <c r="G36" s="2">
+        <v>3.5148494399999999</v>
+      </c>
+      <c r="H36" s="2">
+        <v>3.7159455299999999</v>
+      </c>
+      <c r="I36" s="2">
+        <v>8.9759326599999998</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1.6626186700000001</v>
+      </c>
+      <c r="K36" s="2">
+        <v>1.0557528199999999</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -6299,7 +6984,7 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="C38" s="1"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -6312,7 +6997,6 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -6325,7 +7009,9 @@
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="C40" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -6338,7 +7024,9 @@
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="C41" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -6351,7 +7039,6 @@
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -6364,7 +7051,9 @@
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="C43" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -7819,6 +8508,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>